<commit_message>
Changed coastal to marine
</commit_message>
<xml_diff>
--- a/Data/WBID_criteria.xlsx
+++ b/Data/WBID_criteria.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pinellasgov.sharepoint.com/sites/BCC-PW-ENVMT/Monitoring and Assessment/R/water_quality_dashboard/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="318" documentId="13_ncr:1_{7A309D96-916D-4D0A-99DA-2AF397C66AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1C5E28A-D0A5-4A3F-BC98-970BDB35D7FD}"/>
+  <xr:revisionPtr revIDLastSave="329" documentId="13_ncr:1_{7A309D96-916D-4D0A-99DA-2AF397C66AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8CB9E93-42C5-485D-8794-B41BCA49131D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE13FCFD-69C3-482F-A9D3-58396836E9E2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE13FCFD-69C3-482F-A9D3-58396836E9E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Criteria" sheetId="1" r:id="rId1"/>
     <sheet name="Units" sheetId="5" r:id="rId2"/>
     <sheet name="Sites" sheetId="6" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Criteria!$A$1:$I$74</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="290">
   <si>
     <t>WBID</t>
   </si>
@@ -196,9 +199,6 @@
     <t>1558N</t>
   </si>
   <si>
-    <t>COASTAL</t>
-  </si>
-  <si>
     <t>1558B</t>
   </si>
   <si>
@@ -908,6 +908,9 @@
   </si>
   <si>
     <t>53-06</t>
+  </si>
+  <si>
+    <t>MARINE</t>
   </si>
 </sst>
 </file>
@@ -1286,11 +1289,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CEB8270-E891-48E2-9417-9A696D4AB26E}">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:I28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1311,28 +1312,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1340,7 +1341,7 @@
         <v>1440</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>35</v>
@@ -1366,7 +1367,7 @@
         <v>1474</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1392,7 +1393,7 @@
         <v>1475</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1418,7 +1419,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>35</v>
@@ -1444,10 +1445,10 @@
         <v>1528</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D6" s="1">
         <v>7.6</v>
@@ -1467,7 +1468,7 @@
         <v>1529</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1493,7 +1494,7 @@
         <v>1530</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>35</v>
@@ -1519,7 +1520,7 @@
         <v>1550</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -1545,7 +1546,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>35</v>
@@ -1571,7 +1572,7 @@
         <v>1569</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>35</v>
@@ -1597,7 +1598,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1623,7 +1624,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>35</v>
@@ -1649,7 +1650,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -1675,7 +1676,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>35</v>
@@ -1701,7 +1702,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1727,7 +1728,7 @@
         <v>1633</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>35</v>
@@ -1753,7 +1754,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>35</v>
@@ -1779,7 +1780,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
@@ -1805,10 +1806,10 @@
         <v>1661</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D20" s="1">
         <v>8.5</v>
@@ -1828,7 +1829,7 @@
         <v>1683</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>35</v>
@@ -1854,7 +1855,7 @@
         <v>1696</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -1880,7 +1881,7 @@
         <v>1700</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>35</v>
@@ -1906,10 +1907,10 @@
         <v>8045</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D24" s="1">
         <v>3.1</v>
@@ -1926,10 +1927,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>35</v>
@@ -1955,7 +1956,7 @@
         <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>40</v>
@@ -1981,7 +1982,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
@@ -2004,10 +2005,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>35</v>
@@ -2033,7 +2034,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -2059,10 +2060,10 @@
         <v>48</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D30" s="1">
         <v>8.3000000000000007</v>
@@ -2082,10 +2083,10 @@
         <v>47</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D31" s="1">
         <v>5.4</v>
@@ -2105,7 +2106,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -2131,7 +2132,7 @@
         <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>32</v>
@@ -2157,7 +2158,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -2183,7 +2184,7 @@
         <v>8</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
@@ -2209,7 +2210,7 @@
         <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
@@ -2232,13 +2233,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D37" s="1">
         <v>9.3000000000000007</v>
@@ -2255,13 +2256,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D38" s="1">
         <v>9.3000000000000007</v>
@@ -2281,10 +2282,10 @@
         <v>46</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D39" s="1">
         <v>9.3000000000000007</v>
@@ -2304,10 +2305,10 @@
         <v>45</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D40" s="1">
         <v>9.3000000000000007</v>
@@ -2327,10 +2328,10 @@
         <v>44</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D41" s="1">
         <v>9.3000000000000007</v>
@@ -2347,13 +2348,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D42" s="1">
         <v>9.3000000000000007</v>
@@ -2370,13 +2371,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D43" s="1">
         <v>9.3000000000000007</v>
@@ -2396,10 +2397,10 @@
         <v>51</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D44" s="1">
         <v>6.3</v>
@@ -2419,7 +2420,7 @@
         <v>12</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>32</v>
@@ -2445,7 +2446,7 @@
         <v>14</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -2471,7 +2472,7 @@
         <v>9</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>
@@ -2497,7 +2498,7 @@
         <v>38</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>40</v>
@@ -2523,7 +2524,7 @@
         <v>10</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>32</v>
@@ -2549,7 +2550,7 @@
         <v>28</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>32</v>
@@ -2575,7 +2576,7 @@
         <v>36</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>40</v>
@@ -2601,7 +2602,7 @@
         <v>29</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>32</v>
@@ -2624,22 +2625,22 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>41</v>
+        <v>217</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>125</v>
+        <v>216</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D53" s="1">
         <v>20</v>
       </c>
       <c r="E53" s="1">
-        <v>1.6</v>
+        <v>1.54</v>
       </c>
       <c r="F53" s="1">
-        <v>9.5000000000000001E-2</v>
+        <v>0.12</v>
       </c>
       <c r="G53" s="1">
         <v>38</v>
@@ -2650,10 +2651,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>40</v>
@@ -2676,59 +2677,59 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D55" s="1">
-        <v>8.3000000000000007</v>
+        <v>20</v>
       </c>
       <c r="E55" s="1">
-        <v>0.56999999999999995</v>
+        <v>1.6</v>
       </c>
       <c r="F55" s="1">
-        <v>0.11</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="G55" s="1">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="H55" s="1">
+        <v>410</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>32</v>
+        <v>289</v>
       </c>
       <c r="D56" s="1">
-        <v>20</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E56" s="1">
-        <v>1.54</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F56" s="1">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="G56" s="1">
-        <v>38</v>
-      </c>
-      <c r="H56" s="1">
-        <v>410</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>32</v>
@@ -2751,16 +2752,16 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D58" s="1">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E58" s="1">
         <v>1.54</v>
@@ -2771,22 +2772,22 @@
       <c r="G58" s="1">
         <v>38</v>
       </c>
-      <c r="I58" s="1">
-        <v>130</v>
+      <c r="H58" s="1">
+        <v>410</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D59" s="1">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E59" s="1">
         <v>1.54</v>
@@ -2797,16 +2798,16 @@
       <c r="G59" s="1">
         <v>38</v>
       </c>
-      <c r="H59" s="1">
-        <v>410</v>
+      <c r="I59" s="1">
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>32</v>
@@ -2829,10 +2830,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>32</v>
@@ -2855,10 +2856,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>32</v>
@@ -2881,10 +2882,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>32</v>
@@ -2907,10 +2908,10 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>32</v>
@@ -2933,10 +2934,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>32</v>
@@ -2959,36 +2960,39 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D66" s="1">
-        <v>8.3000000000000007</v>
+        <v>20</v>
       </c>
       <c r="E66" s="1">
-        <v>0.56999999999999995</v>
+        <v>1.54</v>
       </c>
       <c r="F66" s="1">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="G66" s="1">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="H66" s="1">
+        <v>410</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="D67" s="1">
         <v>8.3000000000000007</v>
@@ -3005,42 +3009,39 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>273</v>
+        <v>50</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>272</v>
+        <v>137</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>32</v>
+        <v>289</v>
       </c>
       <c r="D68" s="1">
-        <v>20</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E68" s="1">
-        <v>1.54</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F68" s="1">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="G68" s="1">
-        <v>38</v>
-      </c>
-      <c r="H68" s="1">
-        <v>410</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>35</v>
+        <v>272</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D69" s="1">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E69" s="1">
         <v>1.54</v>
@@ -3051,18 +3052,18 @@
       <c r="G69" s="1">
         <v>38</v>
       </c>
-      <c r="I69" s="1">
-        <v>130</v>
+      <c r="H69" s="1">
+        <v>410</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C70" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D70" s="1">
@@ -3083,10 +3084,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>35</v>
@@ -3109,16 +3110,16 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D72" s="1">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E72" s="1">
         <v>1.54</v>
@@ -3129,22 +3130,22 @@
       <c r="G72" s="1">
         <v>38</v>
       </c>
-      <c r="H72" s="1">
-        <v>410</v>
+      <c r="I72" s="1">
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>280</v>
+        <v>31</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>281</v>
+        <v>140</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D73" s="1">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E73" s="1">
         <v>1.54</v>
@@ -3155,7 +3156,33 @@
       <c r="G73" s="1">
         <v>38</v>
       </c>
-      <c r="I73" s="1">
+      <c r="H73" s="1">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D74" s="1">
+        <v>11</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1.54</v>
+      </c>
+      <c r="F74" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="G74" s="1">
+        <v>38</v>
+      </c>
+      <c r="I74" s="1">
         <v>130</v>
       </c>
     </row>
@@ -3180,50 +3207,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>57</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
         <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3231,7 +3258,7 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3243,9 +3270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446DEF65-5E77-4BAF-B17C-A7715D6429D1}">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3259,10 +3284,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>39</v>
@@ -3271,24 +3296,24 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
         <v>146</v>
-      </c>
-      <c r="F1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E2" s="3">
         <v>28.157197</v>
@@ -3299,16 +3324,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" s="3">
         <v>28.173974999999999</v>
@@ -3319,16 +3344,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="3">
         <v>28.174032</v>
@@ -3339,16 +3364,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
         <v>152</v>
-      </c>
-      <c r="B5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>153</v>
       </c>
       <c r="E5" s="3">
         <v>28.162289999999999</v>
@@ -3359,16 +3384,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
         <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E6" s="3">
         <v>28.151558000000001</v>
@@ -3379,16 +3404,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E7" s="3">
         <v>28.165811999999999</v>
@@ -3399,16 +3424,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
         <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8" s="3">
         <v>28.163824999999999</v>
@@ -3419,16 +3444,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" t="s">
         <v>157</v>
-      </c>
-      <c r="B9" t="s">
-        <v>158</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E9" s="3">
         <v>28.147479000000001</v>
@@ -3439,16 +3464,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E10" s="3">
         <v>28.153013000000001</v>
@@ -3459,16 +3484,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E11" s="4">
         <v>28.148797999999999</v>
@@ -3479,10 +3504,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" t="s">
         <v>162</v>
-      </c>
-      <c r="B12" t="s">
-        <v>163</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
@@ -3499,10 +3524,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
         <v>35</v>
@@ -3519,10 +3544,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
@@ -3539,16 +3564,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
         <v>166</v>
-      </c>
-      <c r="B15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>167</v>
       </c>
       <c r="E15" s="3">
         <v>28.140872000000002</v>
@@ -3559,16 +3584,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E16" s="3">
         <v>28.086324999999999</v>
@@ -3579,16 +3604,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E17" s="3">
         <v>28.076658999999999</v>
@@ -3599,16 +3624,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E18" s="3">
         <v>28.046462999999999</v>
@@ -3619,10 +3644,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" t="s">
         <v>32</v>
@@ -3639,10 +3664,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
         <v>32</v>
@@ -3659,16 +3684,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
         <v>174</v>
-      </c>
-      <c r="B21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>175</v>
       </c>
       <c r="E21" s="3">
         <v>28.068168</v>
@@ -3679,10 +3704,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -3699,10 +3724,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
         <v>32</v>
@@ -3719,10 +3744,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
@@ -3739,10 +3764,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
@@ -3759,10 +3784,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
         <v>32</v>
@@ -3779,10 +3804,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -3799,16 +3824,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
         <v>182</v>
-      </c>
-      <c r="B28" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" t="s">
-        <v>183</v>
       </c>
       <c r="E28" s="3">
         <v>28.04138</v>
@@ -3819,10 +3844,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
         <v>32</v>
@@ -3839,10 +3864,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
         <v>32</v>
@@ -3859,10 +3884,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
         <v>32</v>
@@ -3879,10 +3904,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
         <v>32</v>
@@ -3899,10 +3924,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C33" t="s">
         <v>32</v>
@@ -3919,10 +3944,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
         <v>32</v>
@@ -3939,16 +3964,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35" t="s">
         <v>190</v>
-      </c>
-      <c r="B35" t="s">
-        <v>191</v>
       </c>
       <c r="C35" t="s">
         <v>35</v>
       </c>
       <c r="D35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E35" s="3">
         <v>28.020367</v>
@@ -3959,10 +3984,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
         <v>32</v>
@@ -3979,10 +4004,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C37" t="s">
         <v>32</v>
@@ -3999,10 +4024,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
         <v>32</v>
@@ -4019,10 +4044,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
         <v>32</v>
@@ -4039,10 +4064,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C40" t="s">
         <v>32</v>
@@ -4059,10 +4084,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C41" t="s">
         <v>40</v>
@@ -4079,10 +4104,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
         <v>40</v>
@@ -4099,10 +4124,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
         <v>32</v>
@@ -4119,10 +4144,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C44" t="s">
         <v>32</v>
@@ -4139,10 +4164,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
         <v>32</v>
@@ -4159,10 +4184,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C46" t="s">
         <v>32</v>
@@ -4179,10 +4204,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
         <v>32</v>
@@ -4199,10 +4224,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C48" t="s">
         <v>32</v>
@@ -4219,10 +4244,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
         <v>32</v>
@@ -4239,10 +4264,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C50" t="s">
         <v>32</v>
@@ -4259,10 +4284,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C51" t="s">
         <v>32</v>
@@ -4279,10 +4304,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C52" t="s">
         <v>35</v>
@@ -4299,10 +4324,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
         <v>35</v>
@@ -4319,10 +4344,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C54" t="s">
         <v>35</v>
@@ -4339,10 +4364,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C55" t="s">
         <v>32</v>
@@ -4359,10 +4384,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C56" t="s">
         <v>32</v>
@@ -4379,10 +4404,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C57" t="s">
         <v>32</v>
@@ -4399,16 +4424,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>215</v>
+      </c>
+      <c r="B58" t="s">
         <v>216</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" t="s">
         <v>217</v>
-      </c>
-      <c r="C58" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" t="s">
-        <v>218</v>
       </c>
       <c r="E58" s="3">
         <v>27.927420000000001</v>
@@ -4419,10 +4444,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C59" t="s">
         <v>32</v>
@@ -4439,10 +4464,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C60" t="s">
         <v>32</v>
@@ -4459,10 +4484,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C61" t="s">
         <v>32</v>
@@ -4479,10 +4504,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C62" t="s">
         <v>32</v>
@@ -4499,10 +4524,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C63" t="s">
         <v>32</v>
@@ -4519,10 +4544,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C64" t="s">
         <v>35</v>
@@ -4539,10 +4564,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C65" t="s">
         <v>32</v>
@@ -4559,10 +4584,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C66" t="s">
         <v>32</v>
@@ -4579,10 +4604,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C67" t="s">
         <v>32</v>
@@ -4599,10 +4624,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C68" t="s">
         <v>32</v>
@@ -4619,10 +4644,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B69" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C69" t="s">
         <v>32</v>
@@ -4639,10 +4664,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B70" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C70" t="s">
         <v>32</v>
@@ -4659,10 +4684,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C71" t="s">
         <v>32</v>
@@ -4679,10 +4704,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C72" t="s">
         <v>32</v>
@@ -4699,10 +4724,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C73" t="s">
         <v>32</v>
@@ -4719,10 +4744,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C74" t="s">
         <v>32</v>
@@ -4739,10 +4764,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B75" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C75" t="s">
         <v>32</v>
@@ -4759,10 +4784,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B76" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C76" t="s">
         <v>35</v>
@@ -4779,10 +4804,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C77" t="s">
         <v>35</v>
@@ -4799,10 +4824,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B78" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C78" t="s">
         <v>35</v>
@@ -4819,10 +4844,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C79" t="s">
         <v>35</v>
@@ -4839,10 +4864,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B80" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C80" t="s">
         <v>32</v>
@@ -4859,10 +4884,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B81" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C81" t="s">
         <v>32</v>
@@ -4879,10 +4904,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B82" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C82" t="s">
         <v>32</v>
@@ -4899,10 +4924,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B83" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C83" t="s">
         <v>32</v>
@@ -4919,16 +4944,16 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B84" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C84" t="s">
         <v>35</v>
       </c>
       <c r="D84" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E84" s="3">
         <v>27.903523</v>
@@ -4939,16 +4964,16 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>244</v>
+      </c>
+      <c r="B85" t="s">
         <v>245</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
+        <v>32</v>
+      </c>
+      <c r="D85" t="s">
         <v>246</v>
-      </c>
-      <c r="C85" t="s">
-        <v>32</v>
-      </c>
-      <c r="D85" t="s">
-        <v>247</v>
       </c>
       <c r="E85" s="3">
         <v>27.892914999999999</v>
@@ -4959,10 +4984,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B86" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C86" t="s">
         <v>32</v>
@@ -4979,10 +5004,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B87" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C87" t="s">
         <v>32</v>
@@ -4999,16 +5024,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B88" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C88" t="s">
         <v>32</v>
       </c>
       <c r="D88" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E88" s="3">
         <v>27.8797999999999</v>
@@ -5019,10 +5044,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B89" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C89" t="s">
         <v>32</v>
@@ -5039,16 +5064,16 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B90" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C90" t="s">
         <v>32</v>
       </c>
       <c r="D90" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E90" s="3">
         <v>27.894953000000001</v>
@@ -5059,16 +5084,16 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B91" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C91" t="s">
         <v>35</v>
       </c>
       <c r="D91" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E91" s="3">
         <v>27.90765</v>
@@ -5079,10 +5104,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B92" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C92" t="s">
         <v>32</v>
@@ -5099,10 +5124,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>254</v>
+      </c>
+      <c r="B93" t="s">
         <v>255</v>
-      </c>
-      <c r="B93" t="s">
-        <v>256</v>
       </c>
       <c r="C93" t="s">
         <v>32</v>
@@ -5119,16 +5144,16 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C94" t="s">
         <v>35</v>
       </c>
       <c r="D94" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E94" s="3">
         <v>27.808412000000001</v>
@@ -5139,10 +5164,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>258</v>
+      </c>
+      <c r="B95" t="s">
         <v>259</v>
-      </c>
-      <c r="B95" t="s">
-        <v>260</v>
       </c>
       <c r="C95" t="s">
         <v>32</v>
@@ -5159,10 +5184,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B96" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C96" t="s">
         <v>32</v>
@@ -5179,10 +5204,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B97" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C97" t="s">
         <v>32</v>
@@ -5199,10 +5224,10 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B98" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C98" t="s">
         <v>32</v>
@@ -5219,10 +5244,10 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B99" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C99" t="s">
         <v>32</v>
@@ -5239,10 +5264,10 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B100" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C100" t="s">
         <v>32</v>
@@ -5259,10 +5284,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B101" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C101" t="s">
         <v>32</v>
@@ -5279,10 +5304,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B102" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C102" t="s">
         <v>32</v>
@@ -5299,16 +5324,16 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>267</v>
+      </c>
+      <c r="B103" t="s">
         <v>268</v>
-      </c>
-      <c r="B103" t="s">
-        <v>269</v>
       </c>
       <c r="C103" t="s">
         <v>35</v>
       </c>
       <c r="D103" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E103" s="3">
         <v>27.757975999999999</v>
@@ -5319,16 +5344,16 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>270</v>
+      </c>
+      <c r="B104" t="s">
         <v>271</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
+        <v>32</v>
+      </c>
+      <c r="D104" t="s">
         <v>272</v>
-      </c>
-      <c r="C104" t="s">
-        <v>32</v>
-      </c>
-      <c r="D104" t="s">
-        <v>273</v>
       </c>
       <c r="E104" s="3">
         <v>27.764379999999999</v>
@@ -5339,16 +5364,16 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B105" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C105" t="s">
         <v>35</v>
       </c>
       <c r="D105" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E105" s="3">
         <v>27.760207000000001</v>
@@ -5359,16 +5384,16 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>274</v>
+      </c>
+      <c r="B106" t="s">
+        <v>95</v>
+      </c>
+      <c r="C106" t="s">
+        <v>32</v>
+      </c>
+      <c r="D106" t="s">
         <v>275</v>
-      </c>
-      <c r="B106" t="s">
-        <v>96</v>
-      </c>
-      <c r="C106" t="s">
-        <v>32</v>
-      </c>
-      <c r="D106" t="s">
-        <v>276</v>
       </c>
       <c r="E106" s="3">
         <v>27.760513</v>
@@ -5379,16 +5404,16 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B107" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C107" t="s">
         <v>35</v>
       </c>
       <c r="D107" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E107" s="3">
         <v>27.792266000000001</v>
@@ -5399,10 +5424,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B108" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C108" t="s">
         <v>32</v>
@@ -5419,16 +5444,16 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B109" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C109" t="s">
         <v>35</v>
       </c>
       <c r="D109" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E109" s="3">
         <v>27.748215999999999</v>
@@ -5439,10 +5464,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>282</v>
+      </c>
+      <c r="B110" t="s">
         <v>283</v>
-      </c>
-      <c r="B110" t="s">
-        <v>284</v>
       </c>
       <c r="C110" t="s">
         <v>35</v>
@@ -5459,10 +5484,10 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B111" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C111" t="s">
         <v>35</v>
@@ -5479,16 +5504,16 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>285</v>
+      </c>
+      <c r="B112" t="s">
         <v>286</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
+        <v>35</v>
+      </c>
+      <c r="D112" t="s">
         <v>287</v>
-      </c>
-      <c r="C112" t="s">
-        <v>288</v>
-      </c>
-      <c r="D112" t="s">
-        <v>35</v>
       </c>
       <c r="E112" s="3">
         <v>28.106107999999999</v>
@@ -5499,16 +5524,16 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B113" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C113" t="s">
         <v>35</v>
       </c>
       <c r="D113" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E113" s="3">
         <v>28.106427</v>

</xml_diff>